<commit_message>
Remove VLOOKUP from excel
</commit_message>
<xml_diff>
--- a/data/excel_files_reduced_clean_series/vehicle_data_reduced_clean_series.xlsx
+++ b/data/excel_files_reduced_clean_series/vehicle_data_reduced_clean_series.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="VehicleData" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="MileageBand" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="PriceBands" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,50 +534,35 @@
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>Price Band</t>
+          <t>Mileage Rounded to Nearest 50,000</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>Mileage Rounded to Nearest 50,000</t>
+          <t>Engine Size Rounded</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>Mileage Band</t>
+          <t>Price Filter</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>Engine Size Rounded</t>
+          <t>Mileage Filter</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>Price Filter</t>
+          <t>Engine Size Filter</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>Mileage Filter</t>
+          <t>MPG Filter</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
-        <is>
-          <t>Engine Size Filter</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>Year Filter</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>MPG Filter</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
         <is>
           <t>Master Filter</t>
         </is>
@@ -674,43 +657,31 @@
         <v/>
       </c>
       <c r="W2">
-        <f>VLOOKUP(VehicleData!V2, PriceBands!A:C, 3, False)</f>
+        <f>(ROUNDDOWN((AVERAGE(VehicleData!G2)) / (50000), 0)) * (50000)</f>
         <v/>
       </c>
       <c r="X2">
-        <f>(ROUNDDOWN((AVERAGE(VehicleData!G2)) / (50000), 0)) * (50000)</f>
+        <f>ROUND((AVERAGE(VehicleData!P2)) / (1000), 1)</f>
         <v/>
       </c>
       <c r="Y2">
-        <f>VLOOKUP(VehicleData!X2, MileageBand!A:B, 2, False)</f>
+        <f>IF((AVERAGE(VehicleData!V2)) = (30000), 0, 1)</f>
         <v/>
       </c>
       <c r="Z2">
-        <f>ROUND((AVERAGE(VehicleData!P2)) / (1000), 1)</f>
+        <f>IF((AVERAGE(VehicleData!W2)) &gt; (50000), 0, 1)</f>
         <v/>
       </c>
       <c r="AA2">
-        <f>IF((AVERAGE(VehicleData!V2)) = (30000), 0, 1)</f>
+        <f>IF((AVERAGE(VehicleData!X2)) &gt; (2.5), 0, 1)</f>
         <v/>
       </c>
       <c r="AB2">
-        <f>IF((AVERAGE(VehicleData!X2)) &gt; (50000), 0, 1)</f>
+        <f>IF((AVERAGE(VehicleData!Q2)) &lt; (30), 0, 1)</f>
         <v/>
       </c>
       <c r="AC2">
-        <f>IF((AVERAGE(VehicleData!Z2)) &gt; (2.5), 0, 1)</f>
-        <v/>
-      </c>
-      <c r="AD2">
-        <f>IF((AVERAGE(VehicleData!T2:Z2)) &lt; (2014), 0, 1)</f>
-        <v/>
-      </c>
-      <c r="AE2">
-        <f>IF((AVERAGE(VehicleData!Q2)) &lt; (30), 0, 1)</f>
-        <v/>
-      </c>
-      <c r="AF2">
-        <f>IF((SUM(VehicleData!AA2:AE2)) = (5), 1, 0)</f>
+        <f>IF((SUM(VehicleData!Y2:AB2)) = (4), 1, 0)</f>
         <v/>
       </c>
     </row>
@@ -809,157 +780,32 @@
         <v/>
       </c>
       <c r="W3">
-        <f>VLOOKUP(VehicleData!V3, PriceBands!A:C, 3, False)</f>
+        <f>(ROUNDDOWN((AVERAGE(VehicleData!G3)) / (50000), 0)) * (50000)</f>
         <v/>
       </c>
       <c r="X3">
-        <f>(ROUNDDOWN((AVERAGE(VehicleData!G3)) / (50000), 0)) * (50000)</f>
+        <f>ROUND((AVERAGE(VehicleData!P3)) / (1000), 1)</f>
         <v/>
       </c>
       <c r="Y3">
-        <f>VLOOKUP(VehicleData!X3, MileageBand!A:B, 2, False)</f>
+        <f>IF((AVERAGE(VehicleData!V3)) = (30000), 0, 1)</f>
         <v/>
       </c>
       <c r="Z3">
-        <f>ROUND((AVERAGE(VehicleData!P3)) / (1000), 1)</f>
+        <f>IF((AVERAGE(VehicleData!W3)) &gt; (50000), 0, 1)</f>
         <v/>
       </c>
       <c r="AA3">
-        <f>IF((AVERAGE(VehicleData!V3)) = (30000), 0, 1)</f>
+        <f>IF((AVERAGE(VehicleData!X3)) &gt; (2.5), 0, 1)</f>
         <v/>
       </c>
       <c r="AB3">
-        <f>IF((AVERAGE(VehicleData!X3)) &gt; (50000), 0, 1)</f>
+        <f>IF((AVERAGE(VehicleData!Q3)) &lt; (30), 0, 1)</f>
         <v/>
       </c>
       <c r="AC3">
-        <f>IF((AVERAGE(VehicleData!Z3)) &gt; (2.5), 0, 1)</f>
-        <v/>
-      </c>
-      <c r="AD3">
-        <f>IF((AVERAGE(VehicleData!T3:Z3)) &lt; (2014), 0, 1)</f>
-        <v/>
-      </c>
-      <c r="AE3">
-        <f>IF((AVERAGE(VehicleData!Q3)) &lt; (30), 0, 1)</f>
-        <v/>
-      </c>
-      <c r="AF3">
-        <f>IF((SUM(VehicleData!AA3:AE3)) = (5), 1, 0)</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Mileage Lower Limit</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Mileage Band</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>50000</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Price Band Lower Limit</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Price Band Upper Limit</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Price Band</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>£0-5k</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B3" t="n">
-        <v>10000</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>£5-10k</t>
-        </is>
+        <f>IF((SUM(VehicleData!Y3:AB3)) = (4), 1, 0)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>